<commit_message>
modificaciones en el portatil
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -1,7 +1,25 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Velázquez" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -31,8 +49,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +411,401 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nombre_TPV</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_desc</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Nombre_MdP</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>total_ventas</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total_operaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>857.99</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>563.28</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>1351.34</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>957.52</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>2331.75</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>553.54</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Velázquez</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>1098.34</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
recodificación de funciones (formato)
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Velázquez" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="LOCAL LM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,12 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BAR</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C2" s="1" t="n">
@@ -485,25 +480,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>GLOVO</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>295.5</v>
+        <v>190.6</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BAR</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
@@ -516,25 +506,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>857.99</v>
+        <v>7.2</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
@@ -542,7 +527,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tarde</t>
+          <t>Mañana</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,21 +536,16 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>563.28</v>
+        <v>1915.04</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>46</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C5" s="1" t="n">
@@ -573,30 +553,25 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Tarde</t>
+          <t>Mañana</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>GLOVO</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>73.8</v>
+        <v>4663.5</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>5</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C6" s="1" t="n">
@@ -609,25 +584,20 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1351.34</v>
+        <v>295.5</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C7" s="1" t="n">
@@ -635,30 +605,25 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Mañana</t>
+          <t>Tarde</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>957.52</v>
+        <v>857.99</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C8" s="1" t="n">
@@ -671,25 +636,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>GLOVO</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>95.3</v>
+        <v>563.28</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C9" s="1" t="n">
@@ -702,25 +662,20 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>GLOVO</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>3.6</v>
+        <v>73.8</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C10" s="1" t="n">
@@ -737,21 +692,16 @@
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>2331.75</v>
+        <v>1351.34</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>207</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>BAR</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C11" s="1" t="n">
@@ -764,25 +714,20 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>553.54</v>
+        <v>2196.68</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>50</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>BAR</t>
+          <t>LOCAL LM</t>
         </is>
       </c>
       <c r="C12" s="1" t="n">
@@ -795,14 +740,144 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>1107.08</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>563.28</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>1098.34</v>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>99</v>
+      <c r="F15" s="2" t="n">
+        <v>1351.34</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>857.99</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya solo nos queda convertir tarifas y fichas técnicas
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -470,11 +470,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BAR</t>
-        </is>
-      </c>
       <c r="C2" s="1" t="n">
         <v>45627</v>
       </c>
@@ -501,11 +496,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BAR</t>
-        </is>
-      </c>
       <c r="C3" s="1" t="n">
         <v>45627</v>
       </c>
@@ -532,11 +522,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
       <c r="C4" s="1" t="n">
         <v>45627</v>
       </c>
@@ -563,11 +548,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
       <c r="C5" s="1" t="n">
         <v>45627</v>
       </c>
@@ -594,11 +574,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
       <c r="C6" s="1" t="n">
         <v>45627</v>
       </c>
@@ -625,11 +600,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
       <c r="C7" s="1" t="n">
         <v>45627</v>
       </c>
@@ -656,11 +626,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
       <c r="C8" s="1" t="n">
         <v>45627</v>
       </c>
@@ -687,11 +652,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BAR</t>
-        </is>
-      </c>
       <c r="C9" s="1" t="n">
         <v>45627</v>
       </c>
@@ -718,11 +678,6 @@
           <t>Velázquez</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>BAR</t>
-        </is>
-      </c>
       <c r="C10" s="1" t="n">
         <v>45627</v>
       </c>
@@ -747,11 +702,6 @@
       <c r="A11" t="inlineStr">
         <is>
           <t>Velázquez</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>REMOTO</t>
         </is>
       </c>
       <c r="C11" s="1" t="n">

</xml_diff>

<commit_message>
cambio para la selección por orden de opciones de usaurio
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>352.6</v>
+        <v>4010.85</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>35</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>633.8</v>
+        <v>7933.5</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>57</v>
+        <v>711</v>
       </c>
     </row>
     <row r="4">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>616.17</v>
+        <v>3100.5</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>46</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>1524.33</v>
+        <v>7644.6</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>102</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>871.23</v>
+        <v>7256.88</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>103</v>
+        <v>693</v>
       </c>
     </row>
     <row r="7">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -610,14 +610,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>GLOVO</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>324.9</v>
+        <v>20079.27</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>13</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="8">
@@ -627,23 +627,23 @@
         </is>
       </c>
       <c r="C8" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Mañana</t>
+          <t>Tarde</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>2062.02</v>
+        <v>6324.84</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>192</v>
+        <v>711</v>
       </c>
     </row>
     <row r="9">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="C9" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -662,14 +662,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>GLOVO</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>422.9</v>
+        <v>327.6</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="C10" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -688,14 +688,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1405.02</v>
+        <v>42.3</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>112</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -705,11 +705,11 @@
         </is>
       </c>
       <c r="C11" s="1" t="n">
-        <v>45627</v>
+        <v>45689</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mañana</t>
+          <t>Tarde</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>2564.3</v>
+        <v>16288.2</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>226</v>
+        <v>1386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hemos limpiado un poco el tema de excepciones y creo que Ok la httpexception
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4010.85</v>
+        <v>2673.9</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>450</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>7933.5</v>
+        <v>5289</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>711</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>3100.5</v>
+        <v>2067</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>252</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>7644.6</v>
+        <v>5096.4</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>630</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>7256.88</v>
+        <v>4837.92</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>693</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7">
@@ -614,10 +614,10 @@
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>20079.27</v>
+        <v>13386.18</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>1386</v>
+        <v>924</v>
       </c>
     </row>
     <row r="8">
@@ -640,10 +640,10 @@
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>6324.84</v>
+        <v>4216.56</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>711</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9">
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>327.6</v>
+        <v>218.4</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>42.3</v>
+        <v>28.2</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>16288.2</v>
+        <v>10858.8</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>1386</v>
+        <v>924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorgazación servicios python y mejoras de CHATGPT
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Velázquez" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tienda Velázquez" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +467,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BAR</t>
         </is>
       </c>
       <c r="C2" s="1" t="n">
@@ -493,7 +498,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BAR</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
@@ -519,7 +529,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BAR</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
@@ -545,7 +560,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BAR</t>
         </is>
       </c>
       <c r="C5" s="1" t="n">
@@ -571,7 +591,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C6" s="1" t="n">
@@ -597,7 +622,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C7" s="1" t="n">
@@ -623,7 +653,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C8" s="1" t="n">
@@ -649,7 +684,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C9" s="1" t="n">
@@ -675,7 +715,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C10" s="1" t="n">
@@ -701,7 +746,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Velázquez</t>
+          <t>Tienda Velázquez</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="C11" s="1" t="n">

</xml_diff>

<commit_message>
Hasta arqueo INF y consulta cierre
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tienda Velázquez" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tienda - Velázquez" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,30 +435,35 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>serie</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Nombre_TPV</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>fecha</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>cierre_tpv_desc</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Nombre_MdP</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>total_ventas</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>total_operaciones</t>
         </is>
@@ -467,311 +472,361 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>BAR</t>
         </is>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+      <c r="D2" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>EUROS</t>
         </is>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>2673.9</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>300</v>
+      <c r="G2" s="2" t="n">
+        <v>72.75</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>BAR</t>
         </is>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+      <c r="D3" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>5289</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>474</v>
+      <c r="G3" s="2" t="n">
+        <v>202.1</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>BAR</t>
         </is>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+      <c r="D4" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>EUROS</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>2067</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>168</v>
+      <c r="G4" s="2" t="n">
+        <v>83.40000000000001</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>BAR</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+      <c r="D5" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>5096.4</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>420</v>
+      <c r="G5" s="2" t="n">
+        <v>139.8</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>SERVIDOR TIENDA</t>
         </is>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+      <c r="D6" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>EUROS</t>
         </is>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>4837.92</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>462</v>
+      <c r="G6" s="2" t="n">
+        <v>806.3200000000001</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>SERVIDOR TIENDA</t>
         </is>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+      <c r="D7" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>13386.18</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>924</v>
+      <c r="G7" s="2" t="n">
+        <v>2231.03</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>SERVIDOR TIENDA</t>
         </is>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+      <c r="D8" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>EUROS</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>4216.56</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>474</v>
+      <c r="G8" s="2" t="n">
+        <v>702.76</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>SERVIDOR TIENDA</t>
         </is>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+      <c r="D9" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>GLOVO</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>218.4</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>12</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>SERVIDOR TIENDA</t>
         </is>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+      <c r="D10" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>28.2</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>6</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1809.8</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tienda Velázquez</t>
+          <t>Tienda - Velázquez</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Tarde</t>
-        </is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>45689</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="F11" s="2" t="n">
-        <v>10858.8</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>924</v>
+      <c r="G11" s="2" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OK. todo preprado para poder enseñarlo en el portatil
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,20 +450,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>cierre_tpv_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>cierre_tpv_desc</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Nombre_MdP</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>total_ventas</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>total_operaciones</t>
         </is>
@@ -477,32 +482,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8868</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>72.75</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>9</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -522,23 +530,26 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8869</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>202.1</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>24</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -558,23 +569,26 @@
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8869</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>83.40000000000001</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>9</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>173.7</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -585,32 +599,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8870</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>139.8</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>14</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>573.8</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="6">
@@ -630,23 +647,26 @@
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8870</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>806.3200000000001</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>77</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1134.89</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="7">
@@ -657,32 +677,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8871</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>2231.03</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>154</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>249.3</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -693,32 +716,35 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8871</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>702.76</v>
-      </c>
-      <c r="H8" s="3" t="n">
-        <v>79</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>370.77</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -738,23 +764,26 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8872</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>1</v>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>223.78</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -774,23 +803,26 @@
         </is>
       </c>
       <c r="D10" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8872</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>1809.8</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>154</v>
+      <c r="H10" s="2" t="n">
+        <v>837.98</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="11">
@@ -810,23 +842,26 @@
         </is>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45689</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Mañana</t>
-        </is>
+        <v>45700</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8873</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>93.2</v>
-      </c>
-      <c r="H11" s="3" t="n">
-        <v>13</v>
+      <c r="H11" s="2" t="n">
+        <v>126.2</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Muchos cambios todo Ok
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +465,15 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>total_arqueo_ciego</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>total_ventas</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>total_operaciones</t>
         </is>
@@ -482,19 +487,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E2" t="n">
-        <v>8868</v>
+        <v>8829</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -503,14 +508,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SMS</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>54.5</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>3</v>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>551.3</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>72.75</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -530,10 +538,10 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E3" t="n">
-        <v>8869</v>
+        <v>8829</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -542,14 +550,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>63.5</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>15</v>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>891.6</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>202.1</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -569,10 +580,10 @@
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E4" t="n">
-        <v>8869</v>
+        <v>8830</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -581,14 +592,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>173.7</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>32</v>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>422.05</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>83.40000000000001</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -599,19 +613,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E5" t="n">
-        <v>8870</v>
+        <v>8830</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -620,14 +634,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>573.8</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>82</v>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>867</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>139.8</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -647,10 +664,10 @@
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E6" t="n">
-        <v>8870</v>
+        <v>8828</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -659,14 +676,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>1134.89</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>151</v>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1204.3</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>806.3200000000001</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>77</v>
       </c>
     </row>
     <row r="7">
@@ -677,19 +697,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E7" t="n">
-        <v>8871</v>
+        <v>8828</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -698,14 +718,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>249.3</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>30</v>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2231.23</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>2231.03</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="8">
@@ -716,19 +739,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E8" t="n">
-        <v>8871</v>
+        <v>8831</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -737,14 +760,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>370.77</v>
-      </c>
-      <c r="I8" s="3" t="n">
-        <v>48</v>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>1130.48</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>702.76</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="9">
@@ -764,10 +790,10 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E9" t="n">
-        <v>8872</v>
+        <v>8831</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -776,14 +802,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>EUROS</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>223.78</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>40</v>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -803,10 +832,10 @@
         </is>
       </c>
       <c r="D10" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E10" t="n">
-        <v>8872</v>
+        <v>8831</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -818,11 +847,14 @@
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="H10" s="2" t="n">
-        <v>837.98</v>
-      </c>
-      <c r="I10" s="3" t="n">
-        <v>87</v>
+      <c r="H10" t="n">
+        <v>1801.6</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>1809.8</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="11">
@@ -842,10 +874,10 @@
         </is>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45700</v>
+        <v>45689</v>
       </c>
       <c r="E11" t="n">
-        <v>8873</v>
+        <v>8833</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -857,11 +889,14 @@
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="H11" s="2" t="n">
-        <v>126.2</v>
-      </c>
-      <c r="I11" s="3" t="n">
-        <v>19</v>
+      <c r="H11" t="n">
+        <v>1373</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificaciones varias de mallorquina (ya no se cuales :-) ) pero ahora podemos llamar a un servicio externo
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Tienda - Velázquez" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tienda SOL-Bombonería" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tienda MG" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Tienda MG Norte" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,10 +494,10 @@
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E2" t="n">
-        <v>8868</v>
+        <v>8892</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -503,14 +506,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>54.5</v>
+        <v>170.16</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -521,19 +524,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E3" t="n">
-        <v>8869</v>
+        <v>8892</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -542,14 +545,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>63.5</v>
+        <v>62.3</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -569,10 +572,10 @@
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E4" t="n">
-        <v>8869</v>
+        <v>8893</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -581,14 +584,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>173.7</v>
+        <v>156.4</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -599,19 +602,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E5" t="n">
-        <v>8870</v>
+        <v>8893</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -620,14 +623,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>573.8</v>
+        <v>424.2</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -647,10 +650,10 @@
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E6" t="n">
-        <v>8870</v>
+        <v>8894</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -659,14 +662,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>1134.89</v>
+        <v>585.17</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>151</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
@@ -677,19 +680,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E7" t="n">
-        <v>8871</v>
+        <v>8894</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -698,14 +701,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>249.3</v>
+        <v>4.1</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -716,19 +719,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E8" t="n">
-        <v>8871</v>
+        <v>8894</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -741,10 +744,10 @@
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>370.77</v>
+        <v>1093.11</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>48</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9">
@@ -755,19 +758,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E9" t="n">
-        <v>8872</v>
+        <v>8895</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -780,10 +783,10 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>223.78</v>
+        <v>118.1</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -794,19 +797,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D10" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E10" t="n">
-        <v>8872</v>
+        <v>8895</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -815,14 +818,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>837.98</v>
+        <v>3.5</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>87</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -842,10 +845,10 @@
         </is>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45700</v>
+        <v>45706</v>
       </c>
       <c r="E11" t="n">
-        <v>8873</v>
+        <v>8895</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -858,10 +861,880 @@
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>126.2</v>
+        <v>213.6</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>19</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tienda - Velázquez</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8896</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>1009.97</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>serie</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nombre_TPV</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_desc</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Nombre_MdP</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_ventas</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>total_operaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14436</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>2059.14</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E3" t="n">
+        <v>14436</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>2400.6</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14435</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1497.3</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E5" t="n">
+        <v>14437</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>2636.21</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E6" t="n">
+        <v>14437</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>2126.2</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tienda SOL-Bombonería</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14438</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1462.6</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>serie</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nombre_TPV</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_desc</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Nombre_MdP</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_ventas</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>total_operaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tienda MG</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MORALEJA</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5434</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>117.45</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tienda MG</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MORALEJA</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5434</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>256.3</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tienda MG</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MORALEJA</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5435</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>33.2</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tienda MG</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MORALEJA</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5435</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>194.55</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>serie</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nombre_TPV</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_desc</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Nombre_MdP</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_ventas</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>total_operaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SERVIDOR NORTE</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7194</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>172.65</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SERVIDOR NORTE</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7194</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>348.33</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MN3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TPV III (Barra)</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7195</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MN3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TPV III (Barra)</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E5" t="n">
+        <v>7195</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MN3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TPV III (Barra)</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7197</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>96.40000000000001</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MN3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TPV III (Barra)</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7197</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>180.2</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tienda MG Norte</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SERVIDOR NORTE</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>45706</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7196</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>269.75</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ok Alergenos en HTML
</commit_message>
<xml_diff>
--- a/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/ficheros/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,19 +487,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E2" t="n">
-        <v>8884</v>
+        <v>8877</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -508,17 +508,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SMS</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>488.1</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>1.8</v>
+        <v>38</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -529,19 +529,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SERVIDOR TIENDA</t>
+          <t>BAR</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E3" t="n">
-        <v>8886</v>
+        <v>8877</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -550,17 +550,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>TARJETA VISA</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>844.41</v>
+        <v>597.95</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>444.7</v>
+        <v>100.55</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -580,10 +580,10 @@
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E4" t="n">
-        <v>8886</v>
+        <v>8876</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -592,17 +592,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TARJETA VISA</t>
+          <t>EUROS</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1267.81</v>
+        <v>908.11</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>1266.01</v>
+        <v>488.06</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -613,19 +613,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E5" t="n">
-        <v>8887</v>
+        <v>8876</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -634,17 +634,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>EUROS</t>
+          <t>SMS</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>415.11</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>171.2</v>
+        <v>5.4</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -655,19 +655,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BAR</t>
+          <t>SERVIDOR TIENDA</t>
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E6" t="n">
-        <v>8887</v>
+        <v>8876</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -680,13 +680,13 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>879.01</v>
+        <v>1063.98</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>383.35</v>
+        <v>1084.13</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E7" t="n">
-        <v>8888</v>
+        <v>8879</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -722,13 +722,13 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>1968.16</v>
+        <v>1199.5</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>576.05</v>
+        <v>830.6</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
@@ -748,10 +748,10 @@
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E8" t="n">
-        <v>8888</v>
+        <v>8879</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -764,13 +764,13 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1557.2</v>
+        <v>2825.69</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>784.3</v>
+        <v>2791.89</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>76</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9">
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45704</v>
+        <v>45702</v>
       </c>
       <c r="E9" t="n">
-        <v>8889</v>
+        <v>8878</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -802,17 +802,143 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>646.2</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>189</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Tienda - Velázquez</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BAR</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>45702</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8878</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>TARJETA VISA</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>1741.4</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>377.9</v>
-      </c>
-      <c r="J9" s="3" t="n">
-        <v>58</v>
+      <c r="H10" t="n">
+        <v>1226.39</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>468.34</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tienda - Velázquez</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>45702</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8880</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2161.42</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>685.51</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tienda - Velázquez</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SERVIDOR TIENDA</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>45702</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8880</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>3045.82</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>1528.91</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>